<commit_message>
ICE journey price calculated from real UK gov data from 2021 petrol prices
</commit_message>
<xml_diff>
--- a/Inputs/2021_data_petrol_price.xlsx
+++ b/Inputs/2021_data_petrol_price.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yazzadsukhia/Desktop/DP5_new_mod/DP5_modelling/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69B5CA3F-52EC-0C42-B6FB-E21D2D79153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F84A773-7C8C-5B4D-B2B0-6B9F36924C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{90E6A559-2D50-244C-B598-98050EBC6FC1}"/>
+    <workbookView xWindow="12200" yWindow="1760" windowWidth="27640" windowHeight="16940" xr2:uid="{90E6A559-2D50-244C-B598-98050EBC6FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>ULSD: Pump price (p/litre)</t>
   </si>
@@ -44,18 +44,12 @@
   <si>
     <t xml:space="preserve"> ULSP:  Pump price (p/litre)</t>
   </si>
-  <si>
-    <t>ULSP = Ultra low sulphur unleaded petrol</t>
-  </si>
-  <si>
-    <t>ULSD = Ultra low sulphur diesel</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,11 +70,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -106,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -120,7 +109,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,15 +423,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE093C8-A24D-CF4F-9F59-102C8EEBE576}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="39" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -454,7 +442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44200</v>
       </c>
@@ -465,7 +453,7 @@
         <v>119.967465</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44207</v>
       </c>
@@ -476,7 +464,7 @@
         <v>120.61450400000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44214</v>
       </c>
@@ -486,11 +474,8 @@
       <c r="C4" s="2">
         <v>121.51814499999999</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44221</v>
       </c>
@@ -500,11 +485,8 @@
       <c r="C5" s="2">
         <v>122.704246</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44228</v>
       </c>
@@ -515,7 +497,7 @@
         <v>123.700436</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44235</v>
       </c>
@@ -526,7 +508,7 @@
         <v>124.087524</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44242</v>
       </c>
@@ -537,7 +519,7 @@
         <v>125.005819</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44249</v>
       </c>
@@ -548,7 +530,7 @@
         <v>125.71305400000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44256</v>
       </c>
@@ -559,7 +541,7 @@
         <v>126.62080400000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44263</v>
       </c>
@@ -570,7 +552,7 @@
         <v>127.39864900000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44270</v>
       </c>
@@ -581,7 +563,7 @@
         <v>128.24372499999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44277</v>
       </c>
@@ -592,7 +574,7 @@
         <v>129.01912099999998</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44284</v>
       </c>
@@ -603,7 +585,7 @@
         <v>129.31510800000001</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44291</v>
       </c>
@@ -614,7 +596,7 @@
         <v>129.35074500000002</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44298</v>
       </c>

</xml_diff>